<commit_message>
viewprofile by user rest service is implemented and modified the restcall excel file by Kunal
</commit_message>
<xml_diff>
--- a/Employee_Management_Portal_REST_Calls.xlsx
+++ b/Employee_Management_Portal_REST_Calls.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deshpande_As\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nemade_k\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -116,9 +116,6 @@
     <t>/employeemanagementportal/forgotpassword</t>
   </si>
   <si>
-    <t>Allows user to generate new password</t>
-  </si>
-  <si>
     <t>{empId}</t>
   </si>
   <si>
@@ -137,24 +134,54 @@
     <t>Edits existing employee profile (can be done only by user)</t>
   </si>
   <si>
+    <t>/employeemanagementportal/viewemployee/{empId}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{
+"empName": "Ashish",                                                                                                                   "contact": 7276463883,                                                            "about": "simple",                                                  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"deptId": 7,                                                                "designation": "Associate Software Engineer",                                                  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                                                                           "maritalStatus": "Single",                                              "experience": 0.3                                                              "skills":[HTML,CSS,JS],                                                    "city": "Pune",                                                                    "state": "Maharashtra",                                                  "country": "India",                                                            "zipcode": "411030"
+    }</t>
+    </r>
+  </si>
+  <si>
+    <t>/employeemanagementportal/viewprofile</t>
+  </si>
+  <si>
+    <t>can be done by any user</t>
+  </si>
+  <si>
     <t>{
-"empName": "Ashish",                                                                                                                   "contact": 7276463883,                                                            "about": "simple",                                                  "deptId": 7,                                                                "designation": "Associate Software Engineer",                                                                                                                                                             "maritalStatus": "Single",                                              "experience": 0.3                                                              "skills":[HTML,CSS,JS],                                                    "city": "Pune",                                                                    "state": "Maharashtra",                                                  "country": "India",                                                            "zipcode": "411030"
-    }</t>
-  </si>
-  <si>
-    <t>/employeemanagementportal/viewemployee/{empId}</t>
-  </si>
-  <si>
-    <t>{
-"empId": "X4482",                                  "empName": "Ashish",                                  "email": "ashish@gmail.com",           "password": "xyz",                                                             "empType": "Admin"                                                                       "contact": 12345,                                                            "about": "simple",                                                  "deptId": 7,                                                                "designation": "Associate Software Engineer",   "dob": "02/05/1994",                                                       "joiningDate": "01/08/2016",                                       "status": "unlocked",                                                      "gender": "Male",                                                             "maritalStatus": "Single",                                              "experience": 0.3                                                              "skills":[HTML,CSS,JS],                                                    "city": "Pune",                                                                    "state": "Maharashtra",                                                  "country": "India",                                                            "zipcode": "411030"
-    }</t>
+"name": "Ashish",                                  "email": "ashish@gmail.com",           "password": "xyz",                                                             usertype "Admin"                                                                       "contact": 12345,                                                            "about": "simple",                                                  "departmentId": 7,                                                                "designation": "Associate Software Engg",                                                "dateOfBirth": "02/05/1994",                                                       "dateOfJoining": "01/08/2016",                                                                                        "gender": "Male",                                                             "maritalStatus": "Single",              "lockStatus" : "unlock" ,                                           "experience": 0.3 ,                                                             "skills":{ ["skill":"C++" , "skill":"Java"]}                                                                                                                                       "address": { "city": "Pune", "state": Maharashtra", "country": "India", "zipcode": "411030"},                              "salary" :{"basic":12000 , "hra":12500 , "lta": 1000},                                       "userCredential" : {"username":"xyz", "password":"1234"}                                                               }</t>
+  </si>
+  <si>
+    <t>Generate new Password and sends to user's registered email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,8 +209,15 @@
       <name val="Arial Rounded MT Bold"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,7 +226,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -233,20 +273,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -260,31 +291,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,23 +461,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -458,23 +496,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -653,13 +674,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="16"/>
+    <col min="1" max="1" width="9.140625" style="9"/>
     <col min="3" max="3" width="50.140625" customWidth="1"/>
     <col min="4" max="4" width="32.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
@@ -668,36 +689,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="1:7" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+    </row>
+    <row r="3" spans="1:7" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -719,285 +740,295 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
+    <row r="5" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="330" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" s="13" customFormat="1" ht="360" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>4</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>5</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:7" s="19" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>6</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:7" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>7</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>8</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="1:7" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
+        <v>9</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <v>10</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7" s="19" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <v>11</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
+        <v>12</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="E16" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
-        <v>5</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="14">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <v>7</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
-        <v>9</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
-        <v>10</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" ht="225" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
-        <v>11</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="7"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="7"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="7"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="7"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>